<commit_message>
fix: fix JSON data format
</commit_message>
<xml_diff>
--- a/data/xlsx/DL.xlsx
+++ b/data/xlsx/DL.xlsx
@@ -41,94 +41,94 @@
     <t>deaths</t>
   </si>
   <si>
-    <t>2020-06-30</t>
+    <t>2020-06-01</t>
+  </si>
+  <si>
+    <t>2020-06-02</t>
+  </si>
+  <si>
+    <t>2020-06-03</t>
+  </si>
+  <si>
+    <t>2020-06-04</t>
+  </si>
+  <si>
+    <t>2020-06-05</t>
+  </si>
+  <si>
+    <t>2020-06-06</t>
+  </si>
+  <si>
+    <t>2020-06-07</t>
+  </si>
+  <si>
+    <t>2020-06-08</t>
+  </si>
+  <si>
+    <t>2020-06-09</t>
+  </si>
+  <si>
+    <t>2020-06-10</t>
+  </si>
+  <si>
+    <t>2020-06-11</t>
+  </si>
+  <si>
+    <t>2020-06-12</t>
+  </si>
+  <si>
+    <t>2020-06-13</t>
+  </si>
+  <si>
+    <t>2020-06-14</t>
+  </si>
+  <si>
+    <t>2020-06-15</t>
+  </si>
+  <si>
+    <t>2020-06-16</t>
+  </si>
+  <si>
+    <t>2020-06-17</t>
+  </si>
+  <si>
+    <t>2020-06-18</t>
+  </si>
+  <si>
+    <t>2020-06-19</t>
+  </si>
+  <si>
+    <t>2020-06-20</t>
+  </si>
+  <si>
+    <t>2020-06-21</t>
+  </si>
+  <si>
+    <t>2020-06-22</t>
+  </si>
+  <si>
+    <t>2020-06-23</t>
+  </si>
+  <si>
+    <t>2020-06-24</t>
+  </si>
+  <si>
+    <t>2020-06-25</t>
+  </si>
+  <si>
+    <t>2020-06-26</t>
+  </si>
+  <si>
+    <t>2020-06-27</t>
+  </si>
+  <si>
+    <t>2020-06-28</t>
   </si>
   <si>
     <t>2020-06-29</t>
   </si>
   <si>
-    <t>2020-06-28</t>
-  </si>
-  <si>
-    <t>2020-06-27</t>
-  </si>
-  <si>
-    <t>2020-06-26</t>
-  </si>
-  <si>
-    <t>2020-06-25</t>
-  </si>
-  <si>
-    <t>2020-06-24</t>
-  </si>
-  <si>
-    <t>2020-06-23</t>
-  </si>
-  <si>
-    <t>2020-06-22</t>
-  </si>
-  <si>
-    <t>2020-06-21</t>
-  </si>
-  <si>
-    <t>2020-06-20</t>
-  </si>
-  <si>
-    <t>2020-06-19</t>
-  </si>
-  <si>
-    <t>2020-06-18</t>
-  </si>
-  <si>
-    <t>2020-06-17</t>
-  </si>
-  <si>
-    <t>2020-06-16</t>
-  </si>
-  <si>
-    <t>2020-06-15</t>
-  </si>
-  <si>
-    <t>2020-06-14</t>
-  </si>
-  <si>
-    <t>2020-06-13</t>
-  </si>
-  <si>
-    <t>2020-06-12</t>
-  </si>
-  <si>
-    <t>2020-06-11</t>
-  </si>
-  <si>
-    <t>2020-06-10</t>
-  </si>
-  <si>
-    <t>2020-06-09</t>
-  </si>
-  <si>
-    <t>2020-06-08</t>
-  </si>
-  <si>
-    <t>2020-06-07</t>
-  </si>
-  <si>
-    <t>2020-06-06</t>
-  </si>
-  <si>
-    <t>2020-06-05</t>
-  </si>
-  <si>
-    <t>2020-06-04</t>
-  </si>
-  <si>
-    <t>2020-06-03</t>
-  </si>
-  <si>
-    <t>2020-06-02</t>
-  </si>
-  <si>
-    <t>2020-06-01</t>
+    <t>2020-06-30</t>
   </si>
   <si>
     <t>2020-07-01</t>
@@ -2159,7 +2159,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="n">
-        <v>2199</v>
+        <v/>
       </c>
       <c r="C2" t="n">
         <v/>
@@ -2168,10 +2168,10 @@
         <v/>
       </c>
       <c r="E2" t="n">
-        <v>2113</v>
+        <v/>
       </c>
       <c r="F2" t="n">
-        <v>62</v>
+        <v/>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2179,7 +2179,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="n">
-        <v>2084</v>
+        <v/>
       </c>
       <c r="C3" t="n">
         <v/>
@@ -2188,10 +2188,10 @@
         <v/>
       </c>
       <c r="E3" t="n">
-        <v>3628</v>
+        <v/>
       </c>
       <c r="F3" t="n">
-        <v>57</v>
+        <v/>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2199,7 +2199,7 @@
         <v>8</v>
       </c>
       <c r="B4" t="n">
-        <v>2889</v>
+        <v/>
       </c>
       <c r="C4" t="n">
         <v/>
@@ -2208,10 +2208,10 @@
         <v/>
       </c>
       <c r="E4" t="n">
-        <v>3306</v>
+        <v/>
       </c>
       <c r="F4" t="n">
-        <v>65</v>
+        <v/>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2219,7 +2219,7 @@
         <v>9</v>
       </c>
       <c r="B5" t="n">
-        <v>2948</v>
+        <v/>
       </c>
       <c r="C5" t="n">
         <v/>
@@ -2228,10 +2228,10 @@
         <v/>
       </c>
       <c r="E5" t="n">
-        <v>2210</v>
+        <v/>
       </c>
       <c r="F5" t="n">
-        <v>66</v>
+        <v/>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2239,7 +2239,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="n">
-        <v>3460</v>
+        <v/>
       </c>
       <c r="C6" t="n">
         <v/>
@@ -2248,10 +2248,10 @@
         <v/>
       </c>
       <c r="E6" t="n">
-        <v>2326</v>
+        <v/>
       </c>
       <c r="F6" t="n">
-        <v>63</v>
+        <v/>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2259,7 +2259,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="n">
-        <v>3390</v>
+        <v/>
       </c>
       <c r="C7" t="n">
         <v/>
@@ -2268,10 +2268,10 @@
         <v/>
       </c>
       <c r="E7" t="n">
-        <v>3328</v>
+        <v/>
       </c>
       <c r="F7" t="n">
-        <v>64</v>
+        <v/>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2279,7 +2279,7 @@
         <v>12</v>
       </c>
       <c r="B8" t="n">
-        <v>3788</v>
+        <v/>
       </c>
       <c r="C8" t="n">
         <v/>
@@ -2288,10 +2288,10 @@
         <v/>
       </c>
       <c r="E8" t="n">
-        <v>2124</v>
+        <v/>
       </c>
       <c r="F8" t="n">
-        <v>64</v>
+        <v/>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2299,7 +2299,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="n">
-        <v>3947</v>
+        <v/>
       </c>
       <c r="C9" t="n">
         <v/>
@@ -2308,10 +2308,10 @@
         <v/>
       </c>
       <c r="E9" t="n">
-        <v>2711</v>
+        <v/>
       </c>
       <c r="F9" t="n">
-        <v>68</v>
+        <v/>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2319,7 +2319,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="n">
-        <v>2909</v>
+        <v/>
       </c>
       <c r="C10" t="n">
         <v/>
@@ -2328,10 +2328,10 @@
         <v/>
       </c>
       <c r="E10" t="n">
-        <v>3589</v>
+        <v/>
       </c>
       <c r="F10" t="n">
-        <v>58</v>
+        <v/>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2339,7 +2339,7 @@
         <v>15</v>
       </c>
       <c r="B11" t="n">
-        <v>3000</v>
+        <v/>
       </c>
       <c r="C11" t="n">
         <v/>
@@ -2348,10 +2348,10 @@
         <v/>
       </c>
       <c r="E11" t="n">
-        <v>1719</v>
+        <v/>
       </c>
       <c r="F11" t="n">
-        <v>63</v>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2359,7 +2359,7 @@
         <v>16</v>
       </c>
       <c r="B12" t="n">
-        <v>3630</v>
+        <v/>
       </c>
       <c r="C12" t="n">
         <v/>
@@ -2368,10 +2368,10 @@
         <v/>
       </c>
       <c r="E12" t="n">
-        <v>7725</v>
+        <v/>
       </c>
       <c r="F12" t="n">
-        <v>77</v>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2399,7 +2399,7 @@
         <v>18</v>
       </c>
       <c r="B14" t="n">
-        <v>2877</v>
+        <v/>
       </c>
       <c r="C14" t="n">
         <v/>
@@ -2408,10 +2408,10 @@
         <v/>
       </c>
       <c r="E14" t="n">
-        <v>3884</v>
+        <v/>
       </c>
       <c r="F14" t="n">
-        <v>65</v>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2499,7 +2499,7 @@
         <v>23</v>
       </c>
       <c r="B19" t="n">
-        <v/>
+        <v>2877</v>
       </c>
       <c r="C19" t="n">
         <v/>
@@ -2508,10 +2508,10 @@
         <v/>
       </c>
       <c r="E19" t="n">
-        <v/>
+        <v>3884</v>
       </c>
       <c r="F19" t="n">
-        <v/>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2539,7 +2539,7 @@
         <v>25</v>
       </c>
       <c r="B21" t="n">
-        <v/>
+        <v>3630</v>
       </c>
       <c r="C21" t="n">
         <v/>
@@ -2548,10 +2548,10 @@
         <v/>
       </c>
       <c r="E21" t="n">
-        <v/>
+        <v>7725</v>
       </c>
       <c r="F21" t="n">
-        <v/>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2559,7 +2559,7 @@
         <v>26</v>
       </c>
       <c r="B22" t="n">
-        <v/>
+        <v>3000</v>
       </c>
       <c r="C22" t="n">
         <v/>
@@ -2568,10 +2568,10 @@
         <v/>
       </c>
       <c r="E22" t="n">
-        <v/>
+        <v>1719</v>
       </c>
       <c r="F22" t="n">
-        <v/>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -2579,7 +2579,7 @@
         <v>27</v>
       </c>
       <c r="B23" t="n">
-        <v/>
+        <v>2909</v>
       </c>
       <c r="C23" t="n">
         <v/>
@@ -2588,10 +2588,10 @@
         <v/>
       </c>
       <c r="E23" t="n">
-        <v/>
+        <v>3589</v>
       </c>
       <c r="F23" t="n">
-        <v/>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -2599,7 +2599,7 @@
         <v>28</v>
       </c>
       <c r="B24" t="n">
-        <v/>
+        <v>3947</v>
       </c>
       <c r="C24" t="n">
         <v/>
@@ -2608,10 +2608,10 @@
         <v/>
       </c>
       <c r="E24" t="n">
-        <v/>
+        <v>2711</v>
       </c>
       <c r="F24" t="n">
-        <v/>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -2619,7 +2619,7 @@
         <v>29</v>
       </c>
       <c r="B25" t="n">
-        <v/>
+        <v>3788</v>
       </c>
       <c r="C25" t="n">
         <v/>
@@ -2628,10 +2628,10 @@
         <v/>
       </c>
       <c r="E25" t="n">
-        <v/>
+        <v>2124</v>
       </c>
       <c r="F25" t="n">
-        <v/>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -2639,7 +2639,7 @@
         <v>30</v>
       </c>
       <c r="B26" t="n">
-        <v/>
+        <v>3390</v>
       </c>
       <c r="C26" t="n">
         <v/>
@@ -2648,10 +2648,10 @@
         <v/>
       </c>
       <c r="E26" t="n">
-        <v/>
+        <v>3328</v>
       </c>
       <c r="F26" t="n">
-        <v/>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -2659,7 +2659,7 @@
         <v>31</v>
       </c>
       <c r="B27" t="n">
-        <v/>
+        <v>3460</v>
       </c>
       <c r="C27" t="n">
         <v/>
@@ -2668,10 +2668,10 @@
         <v/>
       </c>
       <c r="E27" t="n">
-        <v/>
+        <v>2326</v>
       </c>
       <c r="F27" t="n">
-        <v/>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -2679,7 +2679,7 @@
         <v>32</v>
       </c>
       <c r="B28" t="n">
-        <v/>
+        <v>2948</v>
       </c>
       <c r="C28" t="n">
         <v/>
@@ -2688,10 +2688,10 @@
         <v/>
       </c>
       <c r="E28" t="n">
-        <v/>
+        <v>2210</v>
       </c>
       <c r="F28" t="n">
-        <v/>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -2699,7 +2699,7 @@
         <v>33</v>
       </c>
       <c r="B29" t="n">
-        <v/>
+        <v>2889</v>
       </c>
       <c r="C29" t="n">
         <v/>
@@ -2708,10 +2708,10 @@
         <v/>
       </c>
       <c r="E29" t="n">
-        <v/>
+        <v>3306</v>
       </c>
       <c r="F29" t="n">
-        <v/>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -2719,7 +2719,7 @@
         <v>34</v>
       </c>
       <c r="B30" t="n">
-        <v/>
+        <v>2084</v>
       </c>
       <c r="C30" t="n">
         <v/>
@@ -2728,10 +2728,10 @@
         <v/>
       </c>
       <c r="E30" t="n">
-        <v/>
+        <v>3628</v>
       </c>
       <c r="F30" t="n">
-        <v/>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -2739,7 +2739,7 @@
         <v>35</v>
       </c>
       <c r="B31" t="n">
-        <v/>
+        <v>2199</v>
       </c>
       <c r="C31" t="n">
         <v/>
@@ -2748,10 +2748,10 @@
         <v/>
       </c>
       <c r="E31" t="n">
-        <v/>
+        <v>2113</v>
       </c>
       <c r="F31" t="n">
-        <v/>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -13252,16 +13252,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B2" t="n">
-        <v>440</v>
+        <v>261</v>
       </c>
       <c r="C2" t="n">
-        <v>432</v>
+        <v>942</v>
       </c>
       <c r="D2" t="n">
-        <v>933</v>
+        <v>1198</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -13269,16 +13269,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B3" t="n">
-        <v>435</v>
+        <v>266</v>
       </c>
       <c r="C3" t="n">
-        <v>308</v>
+        <v>833</v>
       </c>
       <c r="D3" t="n">
-        <v>871</v>
+        <v>1175</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -13286,16 +13286,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="B4" t="n">
-        <v>417</v>
+        <v>280</v>
       </c>
       <c r="C4" t="n">
-        <v>378</v>
+        <v>1082</v>
       </c>
       <c r="D4" t="n">
-        <v>875</v>
+        <v>940</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -13303,16 +13303,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B5" t="n">
-        <v>315</v>
+        <v>280</v>
       </c>
       <c r="C5" t="n">
-        <v>570</v>
+        <v>1041</v>
       </c>
       <c r="D5" t="n">
-        <v>1018</v>
+        <v>974</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -13320,16 +13320,16 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B6" t="n">
-        <v>280</v>
+        <v>315</v>
       </c>
       <c r="C6" t="n">
-        <v>1041</v>
+        <v>570</v>
       </c>
       <c r="D6" t="n">
-        <v>974</v>
+        <v>1018</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -13337,16 +13337,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="B7" t="n">
-        <v>280</v>
+        <v>417</v>
       </c>
       <c r="C7" t="n">
-        <v>1082</v>
+        <v>378</v>
       </c>
       <c r="D7" t="n">
-        <v>940</v>
+        <v>875</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -13354,16 +13354,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="B8" t="n">
-        <v>266</v>
+        <v>435</v>
       </c>
       <c r="C8" t="n">
-        <v>833</v>
+        <v>308</v>
       </c>
       <c r="D8" t="n">
-        <v>1175</v>
+        <v>871</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -13371,16 +13371,16 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B9" t="n">
-        <v>261</v>
+        <v>440</v>
       </c>
       <c r="C9" t="n">
-        <v>942</v>
+        <v>432</v>
       </c>
       <c r="D9" t="n">
-        <v>1198</v>
+        <v>933</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -21395,16 +21395,16 @@
         <v/>
       </c>
       <c r="D2" t="n">
-        <v>58348</v>
+        <v/>
       </c>
       <c r="E2" t="n">
-        <v>2742</v>
+        <v/>
       </c>
       <c r="F2" t="n">
         <v/>
       </c>
       <c r="G2" t="n">
-        <v>26270</v>
+        <v/>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -21418,16 +21418,16 @@
         <v/>
       </c>
       <c r="D3" t="n">
-        <v>56235</v>
+        <v/>
       </c>
       <c r="E3" t="n">
-        <v>2680</v>
+        <v/>
       </c>
       <c r="F3" t="n">
         <v/>
       </c>
       <c r="G3" t="n">
-        <v>26246</v>
+        <v/>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -21441,16 +21441,16 @@
         <v/>
       </c>
       <c r="D4" t="n">
-        <v>52607</v>
+        <v/>
       </c>
       <c r="E4" t="n">
-        <v>2623</v>
+        <v/>
       </c>
       <c r="F4" t="n">
         <v/>
       </c>
       <c r="G4" t="n">
-        <v>27847</v>
+        <v/>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -21464,16 +21464,16 @@
         <v/>
       </c>
       <c r="D5" t="n">
-        <v>49301</v>
+        <v/>
       </c>
       <c r="E5" t="n">
-        <v>2558</v>
+        <v/>
       </c>
       <c r="F5" t="n">
         <v/>
       </c>
       <c r="G5" t="n">
-        <v>28329</v>
+        <v/>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -21487,16 +21487,16 @@
         <v/>
       </c>
       <c r="D6" t="n">
-        <v>47091</v>
+        <v/>
       </c>
       <c r="E6" t="n">
-        <v>2492</v>
+        <v/>
       </c>
       <c r="F6" t="n">
         <v/>
       </c>
       <c r="G6" t="n">
-        <v>27657</v>
+        <v/>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -21510,16 +21510,16 @@
         <v/>
       </c>
       <c r="D7" t="n">
-        <v>44765</v>
+        <v/>
       </c>
       <c r="E7" t="n">
-        <v>2429</v>
+        <v/>
       </c>
       <c r="F7" t="n">
         <v/>
       </c>
       <c r="G7" t="n">
-        <v>26586</v>
+        <v/>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -21533,16 +21533,16 @@
         <v/>
       </c>
       <c r="D8" t="n">
-        <v>41437</v>
+        <v/>
       </c>
       <c r="E8" t="n">
-        <v>2365</v>
+        <v/>
       </c>
       <c r="F8" t="n">
         <v/>
       </c>
       <c r="G8" t="n">
-        <v>26588</v>
+        <v/>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -21556,16 +21556,16 @@
         <v/>
       </c>
       <c r="D9" t="n">
-        <v>39313</v>
+        <v/>
       </c>
       <c r="E9" t="n">
-        <v>2301</v>
+        <v/>
       </c>
       <c r="F9" t="n">
         <v/>
       </c>
       <c r="G9" t="n">
-        <v>24988</v>
+        <v/>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -21579,16 +21579,16 @@
         <v/>
       </c>
       <c r="D10" t="n">
-        <v>36602</v>
+        <v/>
       </c>
       <c r="E10" t="n">
-        <v>2233</v>
+        <v/>
       </c>
       <c r="F10" t="n">
         <v/>
       </c>
       <c r="G10" t="n">
-        <v>23820</v>
+        <v/>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -21602,16 +21602,16 @@
         <v/>
       </c>
       <c r="D11" t="n">
-        <v>33013</v>
+        <v/>
       </c>
       <c r="E11" t="n">
-        <v>2175</v>
+        <v/>
       </c>
       <c r="F11" t="n">
         <v/>
       </c>
       <c r="G11" t="n">
-        <v>24558</v>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -21625,16 +21625,16 @@
         <v/>
       </c>
       <c r="D12" t="n">
-        <v>31294</v>
+        <v/>
       </c>
       <c r="E12" t="n">
-        <v>2112</v>
+        <v/>
       </c>
       <c r="F12" t="n">
         <v/>
       </c>
       <c r="G12" t="n">
-        <v>23340</v>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -21671,16 +21671,16 @@
         <v/>
       </c>
       <c r="D14" t="n">
-        <v>21341</v>
+        <v/>
       </c>
       <c r="E14" t="n">
-        <v>1969</v>
+        <v/>
       </c>
       <c r="F14" t="n">
         <v/>
       </c>
       <c r="G14" t="n">
-        <v>26669</v>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -21786,16 +21786,16 @@
         <v/>
       </c>
       <c r="D19" t="n">
-        <v/>
+        <v>21341</v>
       </c>
       <c r="E19" t="n">
-        <v/>
+        <v>1969</v>
       </c>
       <c r="F19" t="n">
         <v/>
       </c>
       <c r="G19" t="n">
-        <v/>
+        <v>26669</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -21832,16 +21832,16 @@
         <v/>
       </c>
       <c r="D21" t="n">
-        <v/>
+        <v>31294</v>
       </c>
       <c r="E21" t="n">
-        <v/>
+        <v>2112</v>
       </c>
       <c r="F21" t="n">
         <v/>
       </c>
       <c r="G21" t="n">
-        <v/>
+        <v>23340</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -21855,16 +21855,16 @@
         <v/>
       </c>
       <c r="D22" t="n">
-        <v/>
+        <v>33013</v>
       </c>
       <c r="E22" t="n">
-        <v/>
+        <v>2175</v>
       </c>
       <c r="F22" t="n">
         <v/>
       </c>
       <c r="G22" t="n">
-        <v/>
+        <v>24558</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -21878,16 +21878,16 @@
         <v/>
       </c>
       <c r="D23" t="n">
-        <v/>
+        <v>36602</v>
       </c>
       <c r="E23" t="n">
-        <v/>
+        <v>2233</v>
       </c>
       <c r="F23" t="n">
         <v/>
       </c>
       <c r="G23" t="n">
-        <v/>
+        <v>23820</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -21901,16 +21901,16 @@
         <v/>
       </c>
       <c r="D24" t="n">
-        <v/>
+        <v>39313</v>
       </c>
       <c r="E24" t="n">
-        <v/>
+        <v>2301</v>
       </c>
       <c r="F24" t="n">
         <v/>
       </c>
       <c r="G24" t="n">
-        <v/>
+        <v>24988</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -21924,16 +21924,16 @@
         <v/>
       </c>
       <c r="D25" t="n">
-        <v/>
+        <v>41437</v>
       </c>
       <c r="E25" t="n">
-        <v/>
+        <v>2365</v>
       </c>
       <c r="F25" t="n">
         <v/>
       </c>
       <c r="G25" t="n">
-        <v/>
+        <v>26588</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -21947,16 +21947,16 @@
         <v/>
       </c>
       <c r="D26" t="n">
-        <v/>
+        <v>44765</v>
       </c>
       <c r="E26" t="n">
-        <v/>
+        <v>2429</v>
       </c>
       <c r="F26" t="n">
         <v/>
       </c>
       <c r="G26" t="n">
-        <v/>
+        <v>26586</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -21970,16 +21970,16 @@
         <v/>
       </c>
       <c r="D27" t="n">
-        <v/>
+        <v>47091</v>
       </c>
       <c r="E27" t="n">
-        <v/>
+        <v>2492</v>
       </c>
       <c r="F27" t="n">
         <v/>
       </c>
       <c r="G27" t="n">
-        <v/>
+        <v>27657</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -21993,16 +21993,16 @@
         <v/>
       </c>
       <c r="D28" t="n">
-        <v/>
+        <v>49301</v>
       </c>
       <c r="E28" t="n">
-        <v/>
+        <v>2558</v>
       </c>
       <c r="F28" t="n">
         <v/>
       </c>
       <c r="G28" t="n">
-        <v/>
+        <v>28329</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -22016,16 +22016,16 @@
         <v/>
       </c>
       <c r="D29" t="n">
-        <v/>
+        <v>52607</v>
       </c>
       <c r="E29" t="n">
-        <v/>
+        <v>2623</v>
       </c>
       <c r="F29" t="n">
         <v/>
       </c>
       <c r="G29" t="n">
-        <v/>
+        <v>27847</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -22039,16 +22039,16 @@
         <v/>
       </c>
       <c r="D30" t="n">
-        <v/>
+        <v>56235</v>
       </c>
       <c r="E30" t="n">
-        <v/>
+        <v>2680</v>
       </c>
       <c r="F30" t="n">
         <v/>
       </c>
       <c r="G30" t="n">
-        <v/>
+        <v>26246</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -22062,16 +22062,16 @@
         <v/>
       </c>
       <c r="D31" t="n">
-        <v/>
+        <v>58348</v>
       </c>
       <c r="E31" t="n">
-        <v/>
+        <v>2742</v>
       </c>
       <c r="F31" t="n">
         <v/>
       </c>
       <c r="G31" t="n">
-        <v/>
+        <v>26270</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -34159,422 +34159,422 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B2" t="n">
-        <v>13661</v>
+        <v>10919</v>
       </c>
       <c r="C2" t="n">
-        <v>5912</v>
+        <v>5448</v>
       </c>
       <c r="D2" t="n">
-        <v>7749</v>
+        <v>5471</v>
       </c>
       <c r="E2" t="n">
-        <v>7869</v>
+        <v>344</v>
       </c>
       <c r="F2" t="n">
-        <v>1686</v>
+        <v>140</v>
       </c>
       <c r="G2" t="n">
-        <v>6183</v>
+        <v>204</v>
       </c>
       <c r="H2" t="n">
-        <v>544</v>
+        <v>5974</v>
       </c>
       <c r="I2" t="n">
-        <v>233</v>
+        <v>1155</v>
       </c>
       <c r="J2" t="n">
-        <v>311</v>
+        <v>4819</v>
       </c>
       <c r="K2" t="n">
-        <v>16240</v>
+        <v/>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B3" t="n">
-        <v>13411</v>
+        <v>12208</v>
       </c>
       <c r="C3" t="n">
-        <v>5977</v>
+        <v>5923</v>
       </c>
       <c r="D3" t="n">
-        <v>7434</v>
+        <v>6285</v>
       </c>
       <c r="E3" t="n">
-        <v>7869</v>
+        <v>5909</v>
       </c>
       <c r="F3" t="n">
-        <v>1615</v>
+        <v>1139</v>
       </c>
       <c r="G3" t="n">
-        <v>6254</v>
+        <v>4770</v>
       </c>
       <c r="H3" t="n">
-        <v>544</v>
+        <v>344</v>
       </c>
       <c r="I3" t="n">
-        <v>241</v>
+        <v>149</v>
       </c>
       <c r="J3" t="n">
-        <v>303</v>
+        <v>195</v>
       </c>
       <c r="K3" t="n">
-        <v>16329</v>
+        <v>12611</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B4" t="n">
-        <v>13411</v>
+        <v>12651</v>
       </c>
       <c r="C4" t="n">
-        <v>6014</v>
+        <v>6054</v>
       </c>
       <c r="D4" t="n">
-        <v>7397</v>
+        <v>6597</v>
       </c>
       <c r="E4" t="n">
         <v>5909</v>
       </c>
       <c r="F4" t="n">
-        <v>1558</v>
+        <v>1426</v>
       </c>
       <c r="G4" t="n">
-        <v>4351</v>
+        <v>4883</v>
       </c>
       <c r="H4" t="n">
         <v>344</v>
       </c>
       <c r="I4" t="n">
-        <v>238</v>
+        <v>205</v>
       </c>
       <c r="J4" t="n">
-        <v>106</v>
+        <v>139</v>
       </c>
       <c r="K4" t="n">
-        <v>17148</v>
+        <v>12106</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B5" t="n">
-        <v>13411</v>
+        <v>13183</v>
       </c>
       <c r="C5" t="n">
-        <v>6068</v>
+        <v>6213</v>
       </c>
       <c r="D5" t="n">
-        <v>7343</v>
+        <v>6970</v>
       </c>
       <c r="E5" t="n">
         <v>5909</v>
       </c>
       <c r="F5" t="n">
-        <v>1700</v>
+        <v>1579</v>
       </c>
       <c r="G5" t="n">
-        <v>4209</v>
+        <v>4330</v>
       </c>
       <c r="H5" t="n">
         <v>344</v>
       </c>
       <c r="I5" t="n">
-        <v>232</v>
+        <v>197</v>
       </c>
       <c r="J5" t="n">
-        <v>112</v>
+        <v>147</v>
       </c>
       <c r="K5" t="n">
-        <v>17381</v>
+        <v>12922</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B6" t="n">
-        <v>13411</v>
+        <v>13389</v>
       </c>
       <c r="C6" t="n">
-        <v>6221</v>
+        <v>6264</v>
       </c>
       <c r="D6" t="n">
-        <v>7190</v>
+        <v>7125</v>
       </c>
       <c r="E6" t="n">
         <v>5909</v>
       </c>
       <c r="F6" t="n">
-        <v>1504</v>
+        <v>1607</v>
       </c>
       <c r="G6" t="n">
-        <v>4405</v>
+        <v>4302</v>
       </c>
       <c r="H6" t="n">
         <v>344</v>
       </c>
       <c r="I6" t="n">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="J6" t="n">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="K6" t="n">
-        <v>16249</v>
+        <v>12963</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B7" t="n">
         <v>13411</v>
       </c>
       <c r="C7" t="n">
-        <v>6241</v>
+        <v>6203</v>
       </c>
       <c r="D7" t="n">
-        <v>7170</v>
+        <v>7208</v>
       </c>
       <c r="E7" t="n">
         <v>5909</v>
       </c>
       <c r="F7" t="n">
-        <v>1585</v>
+        <v>1547</v>
       </c>
       <c r="G7" t="n">
-        <v>4324</v>
+        <v>4362</v>
       </c>
       <c r="H7" t="n">
         <v>344</v>
       </c>
       <c r="I7" t="n">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="J7" t="n">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="K7" t="n">
-        <v>15159</v>
+        <v>14844</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B8" t="n">
         <v>13411</v>
       </c>
       <c r="C8" t="n">
-        <v>6203</v>
+        <v>6241</v>
       </c>
       <c r="D8" t="n">
-        <v>7208</v>
+        <v>7170</v>
       </c>
       <c r="E8" t="n">
         <v>5909</v>
       </c>
       <c r="F8" t="n">
-        <v>1547</v>
+        <v>1585</v>
       </c>
       <c r="G8" t="n">
-        <v>4362</v>
+        <v>4324</v>
       </c>
       <c r="H8" t="n">
         <v>344</v>
       </c>
       <c r="I8" t="n">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="J8" t="n">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="K8" t="n">
-        <v>14844</v>
+        <v>15159</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="B9" t="n">
-        <v>13389</v>
+        <v>13411</v>
       </c>
       <c r="C9" t="n">
-        <v>6264</v>
+        <v>6221</v>
       </c>
       <c r="D9" t="n">
-        <v>7125</v>
+        <v>7190</v>
       </c>
       <c r="E9" t="n">
         <v>5909</v>
       </c>
       <c r="F9" t="n">
-        <v>1607</v>
+        <v>1504</v>
       </c>
       <c r="G9" t="n">
-        <v>4302</v>
+        <v>4405</v>
       </c>
       <c r="H9" t="n">
         <v>344</v>
       </c>
       <c r="I9" t="n">
-        <v>207</v>
+        <v>223</v>
       </c>
       <c r="J9" t="n">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="K9" t="n">
-        <v>12963</v>
+        <v>16249</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B10" t="n">
-        <v>13183</v>
+        <v>13411</v>
       </c>
       <c r="C10" t="n">
-        <v>6213</v>
+        <v>6068</v>
       </c>
       <c r="D10" t="n">
-        <v>6970</v>
+        <v>7343</v>
       </c>
       <c r="E10" t="n">
         <v>5909</v>
       </c>
       <c r="F10" t="n">
-        <v>1579</v>
+        <v>1700</v>
       </c>
       <c r="G10" t="n">
-        <v>4330</v>
+        <v>4209</v>
       </c>
       <c r="H10" t="n">
         <v>344</v>
       </c>
       <c r="I10" t="n">
-        <v>197</v>
+        <v>232</v>
       </c>
       <c r="J10" t="n">
-        <v>147</v>
+        <v>112</v>
       </c>
       <c r="K10" t="n">
-        <v>12922</v>
+        <v>17381</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B11" t="n">
-        <v>12651</v>
+        <v>13411</v>
       </c>
       <c r="C11" t="n">
-        <v>6054</v>
+        <v>6014</v>
       </c>
       <c r="D11" t="n">
-        <v>6597</v>
+        <v>7397</v>
       </c>
       <c r="E11" t="n">
         <v>5909</v>
       </c>
       <c r="F11" t="n">
-        <v>1426</v>
+        <v>1558</v>
       </c>
       <c r="G11" t="n">
-        <v>4883</v>
+        <v>4351</v>
       </c>
       <c r="H11" t="n">
         <v>344</v>
       </c>
       <c r="I11" t="n">
-        <v>205</v>
+        <v>238</v>
       </c>
       <c r="J11" t="n">
-        <v>139</v>
+        <v>106</v>
       </c>
       <c r="K11" t="n">
-        <v>12106</v>
+        <v>17148</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="B12" t="n">
-        <v>12208</v>
+        <v>13411</v>
       </c>
       <c r="C12" t="n">
-        <v>5923</v>
+        <v>5977</v>
       </c>
       <c r="D12" t="n">
-        <v>6285</v>
+        <v>7434</v>
       </c>
       <c r="E12" t="n">
-        <v>5909</v>
+        <v>7869</v>
       </c>
       <c r="F12" t="n">
-        <v>1139</v>
+        <v>1615</v>
       </c>
       <c r="G12" t="n">
-        <v>4770</v>
+        <v>6254</v>
       </c>
       <c r="H12" t="n">
-        <v>344</v>
+        <v>544</v>
       </c>
       <c r="I12" t="n">
-        <v>149</v>
+        <v>241</v>
       </c>
       <c r="J12" t="n">
-        <v>195</v>
+        <v>303</v>
       </c>
       <c r="K12" t="n">
-        <v>12611</v>
+        <v>16329</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="B13" t="n">
-        <v>10919</v>
+        <v>13661</v>
       </c>
       <c r="C13" t="n">
-        <v>5448</v>
+        <v>5912</v>
       </c>
       <c r="D13" t="n">
-        <v>5471</v>
+        <v>7749</v>
       </c>
       <c r="E13" t="n">
-        <v>344</v>
+        <v>7869</v>
       </c>
       <c r="F13" t="n">
-        <v>140</v>
+        <v>1686</v>
       </c>
       <c r="G13" t="n">
-        <v>204</v>
+        <v>6183</v>
       </c>
       <c r="H13" t="n">
-        <v>5974</v>
+        <v>544</v>
       </c>
       <c r="I13" t="n">
-        <v>1155</v>
+        <v>233</v>
       </c>
       <c r="J13" t="n">
-        <v>4819</v>
+        <v>311</v>
       </c>
       <c r="K13" t="n">
-        <v/>
+        <v>16240</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -52115,36 +52115,36 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="B2" t="n">
-        <v>9585</v>
+        <v>9619</v>
       </c>
       <c r="C2" t="n">
-        <v>7594</v>
+        <v>6538</v>
       </c>
       <c r="D2" t="n">
-        <v>531752</v>
+        <v>514573</v>
       </c>
       <c r="E2" t="n">
-        <v>27986</v>
+        <v>27089</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="B3" t="n">
-        <v>9619</v>
+        <v>9585</v>
       </c>
       <c r="C3" t="n">
-        <v>6538</v>
+        <v>7594</v>
       </c>
       <c r="D3" t="n">
-        <v>514573</v>
+        <v>531752</v>
       </c>
       <c r="E3" t="n">
-        <v>27089</v>
+        <v>27986</v>
       </c>
     </row>
     <row r="4" spans="1:5">

</xml_diff>

<commit_message>
data: update csv, json, xlsx data
</commit_message>
<xml_diff>
--- a/data/xlsx/DL.xlsx
+++ b/data/xlsx/DL.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F554"/>
+  <dimension ref="A1:F566"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12623,6 +12623,270 @@
       </c>
       <c r="F554" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>2021-12-10</t>
+        </is>
+      </c>
+      <c r="B555" t="n">
+        <v>41</v>
+      </c>
+      <c r="C555" t="n">
+        <v>59763</v>
+      </c>
+      <c r="D555" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="E555" t="n">
+        <v>57</v>
+      </c>
+      <c r="F555" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>2021-12-11</t>
+        </is>
+      </c>
+      <c r="B556" t="n">
+        <v>52</v>
+      </c>
+      <c r="C556" t="n">
+        <v>57144</v>
+      </c>
+      <c r="D556" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="E556" t="n">
+        <v>37</v>
+      </c>
+      <c r="F556" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>2021-12-12</t>
+        </is>
+      </c>
+      <c r="B557" t="n">
+        <v>56</v>
+      </c>
+      <c r="C557" t="n">
+        <v>56274</v>
+      </c>
+      <c r="D557" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E557" t="n">
+        <v>44</v>
+      </c>
+      <c r="F557" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>2021-12-13</t>
+        </is>
+      </c>
+      <c r="B558" t="n">
+        <v>30</v>
+      </c>
+      <c r="C558" t="n">
+        <v>46169</v>
+      </c>
+      <c r="D558" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="E558" t="n">
+        <v>34</v>
+      </c>
+      <c r="F558" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>2021-12-14</t>
+        </is>
+      </c>
+      <c r="B559" t="n">
+        <v>45</v>
+      </c>
+      <c r="C559" t="n">
+        <v>48120</v>
+      </c>
+      <c r="D559" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="E559" t="n">
+        <v>31</v>
+      </c>
+      <c r="F559" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>2021-12-15</t>
+        </is>
+      </c>
+      <c r="B560" t="n">
+        <v>57</v>
+      </c>
+      <c r="C560" t="n">
+        <v>58328</v>
+      </c>
+      <c r="D560" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E560" t="n">
+        <v>36</v>
+      </c>
+      <c r="F560" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>2021-12-16</t>
+        </is>
+      </c>
+      <c r="B561" t="n">
+        <v>85</v>
+      </c>
+      <c r="C561" t="n">
+        <v>56027</v>
+      </c>
+      <c r="D561" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="E561" t="n">
+        <v>38</v>
+      </c>
+      <c r="F561" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>2021-12-17</t>
+        </is>
+      </c>
+      <c r="B562" t="n">
+        <v>69</v>
+      </c>
+      <c r="C562" t="n">
+        <v>57298</v>
+      </c>
+      <c r="D562" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="E562" t="n">
+        <v>78</v>
+      </c>
+      <c r="F562" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>2021-12-18</t>
+        </is>
+      </c>
+      <c r="B563" t="n">
+        <v>86</v>
+      </c>
+      <c r="C563" t="n">
+        <v>66096</v>
+      </c>
+      <c r="D563" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="E563" t="n">
+        <v>68</v>
+      </c>
+      <c r="F563" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>2021-12-19</t>
+        </is>
+      </c>
+      <c r="B564" t="n">
+        <v>107</v>
+      </c>
+      <c r="C564" t="n">
+        <v>61905</v>
+      </c>
+      <c r="D564" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="E564" t="n">
+        <v>50</v>
+      </c>
+      <c r="F564" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>2021-12-20</t>
+        </is>
+      </c>
+      <c r="B565" t="n">
+        <v>91</v>
+      </c>
+      <c r="C565" t="n">
+        <v>46193</v>
+      </c>
+      <c r="D565" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E565" t="n">
+        <v>100</v>
+      </c>
+      <c r="F565" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>2021-12-21</t>
+        </is>
+      </c>
+      <c r="B566" t="n">
+        <v>102</v>
+      </c>
+      <c r="C566" t="n">
+        <v>51544</v>
+      </c>
+      <c r="D566" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E566" t="n">
+        <v>75</v>
+      </c>
+      <c r="F566" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -12636,7 +12900,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E477"/>
+  <dimension ref="A1:E489"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21712,6 +21976,234 @@
         <v>1437</v>
       </c>
       <c r="E477" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>2021-12-10</t>
+        </is>
+      </c>
+      <c r="B478" t="n">
+        <v>98</v>
+      </c>
+      <c r="C478" t="n">
+        <v>795</v>
+      </c>
+      <c r="D478" t="n">
+        <v>1559</v>
+      </c>
+      <c r="E478" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>2021-12-11</t>
+        </is>
+      </c>
+      <c r="B479" t="n">
+        <v>109</v>
+      </c>
+      <c r="C479" t="n">
+        <v>743</v>
+      </c>
+      <c r="D479" t="n">
+        <v>1515</v>
+      </c>
+      <c r="E479" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>2021-12-12</t>
+        </is>
+      </c>
+      <c r="B480" t="n">
+        <v>113</v>
+      </c>
+      <c r="C480" t="n">
+        <v>641</v>
+      </c>
+      <c r="D480" t="n">
+        <v>1498</v>
+      </c>
+      <c r="E480" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>2021-12-13</t>
+        </is>
+      </c>
+      <c r="B481" t="n">
+        <v>119</v>
+      </c>
+      <c r="C481" t="n">
+        <v>312</v>
+      </c>
+      <c r="D481" t="n">
+        <v>1078</v>
+      </c>
+      <c r="E481" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>2021-12-14</t>
+        </is>
+      </c>
+      <c r="B482" t="n">
+        <v>125</v>
+      </c>
+      <c r="C482" t="n">
+        <v>673</v>
+      </c>
+      <c r="D482" t="n">
+        <v>1709</v>
+      </c>
+      <c r="E482" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>2021-12-15</t>
+        </is>
+      </c>
+      <c r="B483" t="n">
+        <v>128</v>
+      </c>
+      <c r="C483" t="n">
+        <v>851</v>
+      </c>
+      <c r="D483" t="n">
+        <v>1614</v>
+      </c>
+      <c r="E483" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>2021-12-16</t>
+        </is>
+      </c>
+      <c r="B484" t="n">
+        <v>135</v>
+      </c>
+      <c r="C484" t="n">
+        <v>525</v>
+      </c>
+      <c r="D484" t="n">
+        <v>1612</v>
+      </c>
+      <c r="E484" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>2021-12-17</t>
+        </is>
+      </c>
+      <c r="B485" t="n">
+        <v>145</v>
+      </c>
+      <c r="C485" t="n">
+        <v>660</v>
+      </c>
+      <c r="D485" t="n">
+        <v>1571</v>
+      </c>
+      <c r="E485" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>2021-12-18</t>
+        </is>
+      </c>
+      <c r="B486" t="n">
+        <v>153</v>
+      </c>
+      <c r="C486" t="n">
+        <v>719</v>
+      </c>
+      <c r="D486" t="n">
+        <v>1581</v>
+      </c>
+      <c r="E486" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>2021-12-19</t>
+        </is>
+      </c>
+      <c r="B487" t="n">
+        <v>157</v>
+      </c>
+      <c r="C487" t="n">
+        <v>702</v>
+      </c>
+      <c r="D487" t="n">
+        <v>1528</v>
+      </c>
+      <c r="E487" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>2021-12-20</t>
+        </is>
+      </c>
+      <c r="B488" t="n">
+        <v>163</v>
+      </c>
+      <c r="C488" t="n">
+        <v>334</v>
+      </c>
+      <c r="D488" t="n">
+        <v>1186</v>
+      </c>
+      <c r="E488" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>2021-12-21</t>
+        </is>
+      </c>
+      <c r="B489" t="n">
+        <v>173</v>
+      </c>
+      <c r="C489" t="n">
+        <v>801</v>
+      </c>
+      <c r="D489" t="n">
+        <v>1592</v>
+      </c>
+      <c r="E489" t="n">
         <v>0</v>
       </c>
     </row>
@@ -21726,7 +22218,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G554"/>
+  <dimension ref="A1:G566"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -35594,6 +36086,306 @@
       </c>
       <c r="G554" t="n">
         <v>386</v>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>2021-12-10</t>
+        </is>
+      </c>
+      <c r="B555" t="n">
+        <v>1441610</v>
+      </c>
+      <c r="C555" t="n">
+        <v>4.58</v>
+      </c>
+      <c r="D555" t="n">
+        <v>1416140</v>
+      </c>
+      <c r="E555" t="n">
+        <v>25100</v>
+      </c>
+      <c r="F555" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="G555" t="n">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>2021-12-11</t>
+        </is>
+      </c>
+      <c r="B556" t="n">
+        <v>1441662</v>
+      </c>
+      <c r="C556" t="n">
+        <v>4.57</v>
+      </c>
+      <c r="D556" t="n">
+        <v>1416177</v>
+      </c>
+      <c r="E556" t="n">
+        <v>25100</v>
+      </c>
+      <c r="F556" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="G556" t="n">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>2021-12-12</t>
+        </is>
+      </c>
+      <c r="B557" t="n">
+        <v>1441718</v>
+      </c>
+      <c r="C557" t="n">
+        <v>4.56</v>
+      </c>
+      <c r="D557" t="n">
+        <v>1416221</v>
+      </c>
+      <c r="E557" t="n">
+        <v>25100</v>
+      </c>
+      <c r="F557" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="G557" t="n">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>2021-12-13</t>
+        </is>
+      </c>
+      <c r="B558" t="n">
+        <v>1441748</v>
+      </c>
+      <c r="C558" t="n">
+        <v>4.55</v>
+      </c>
+      <c r="D558" t="n">
+        <v>1416255</v>
+      </c>
+      <c r="E558" t="n">
+        <v>25100</v>
+      </c>
+      <c r="F558" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="G558" t="n">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>2021-12-14</t>
+        </is>
+      </c>
+      <c r="B559" t="n">
+        <v>1441793</v>
+      </c>
+      <c r="C559" t="n">
+        <v>4.55</v>
+      </c>
+      <c r="D559" t="n">
+        <v>1416286</v>
+      </c>
+      <c r="E559" t="n">
+        <v>25100</v>
+      </c>
+      <c r="F559" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="G559" t="n">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>2021-12-15</t>
+        </is>
+      </c>
+      <c r="B560" t="n">
+        <v>1441850</v>
+      </c>
+      <c r="C560" t="n">
+        <v>4.54</v>
+      </c>
+      <c r="D560" t="n">
+        <v>1416322</v>
+      </c>
+      <c r="E560" t="n">
+        <v>25100</v>
+      </c>
+      <c r="F560" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="G560" t="n">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>2021-12-16</t>
+        </is>
+      </c>
+      <c r="B561" t="n">
+        <v>1441935</v>
+      </c>
+      <c r="C561" t="n">
+        <v>4.53</v>
+      </c>
+      <c r="D561" t="n">
+        <v>1416360</v>
+      </c>
+      <c r="E561" t="n">
+        <v>25100</v>
+      </c>
+      <c r="F561" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="G561" t="n">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>2021-12-17</t>
+        </is>
+      </c>
+      <c r="B562" t="n">
+        <v>1442004</v>
+      </c>
+      <c r="C562" t="n">
+        <v>4.52</v>
+      </c>
+      <c r="D562" t="n">
+        <v>1416438</v>
+      </c>
+      <c r="E562" t="n">
+        <v>25100</v>
+      </c>
+      <c r="F562" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="G562" t="n">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>2021-12-18</t>
+        </is>
+      </c>
+      <c r="B563" t="n">
+        <v>1442090</v>
+      </c>
+      <c r="C563" t="n">
+        <v>4.51</v>
+      </c>
+      <c r="D563" t="n">
+        <v>1416506</v>
+      </c>
+      <c r="E563" t="n">
+        <v>25100</v>
+      </c>
+      <c r="F563" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="G563" t="n">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>2021-12-19</t>
+        </is>
+      </c>
+      <c r="B564" t="n">
+        <v>1442197</v>
+      </c>
+      <c r="C564" t="n">
+        <v>4.51</v>
+      </c>
+      <c r="D564" t="n">
+        <v>1416556</v>
+      </c>
+      <c r="E564" t="n">
+        <v>25101</v>
+      </c>
+      <c r="F564" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="G564" t="n">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>2021-12-20</t>
+        </is>
+      </c>
+      <c r="B565" t="n">
+        <v>1442288</v>
+      </c>
+      <c r="C565" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D565" t="n">
+        <v>1416656</v>
+      </c>
+      <c r="E565" t="n">
+        <v>25101</v>
+      </c>
+      <c r="F565" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="G565" t="n">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>2021-12-21</t>
+        </is>
+      </c>
+      <c r="B566" t="n">
+        <v>1442390</v>
+      </c>
+      <c r="C566" t="n">
+        <v>4.49</v>
+      </c>
+      <c r="D566" t="n">
+        <v>1416731</v>
+      </c>
+      <c r="E566" t="n">
+        <v>25102</v>
+      </c>
+      <c r="F566" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="G566" t="n">
+        <v>557</v>
       </c>
     </row>
   </sheetData>
@@ -35607,7 +36399,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K513"/>
+  <dimension ref="A1:K525"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -54614,6 +55406,450 @@
       </c>
       <c r="K513" t="n">
         <v>165</v>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>2021-12-10</t>
+        </is>
+      </c>
+      <c r="B514" t="n">
+        <v>9009</v>
+      </c>
+      <c r="C514" t="n">
+        <v>160</v>
+      </c>
+      <c r="D514" t="n">
+        <v>8849</v>
+      </c>
+      <c r="E514" t="n">
+        <v>3871</v>
+      </c>
+      <c r="F514" t="n">
+        <v>0</v>
+      </c>
+      <c r="G514" t="n">
+        <v>3871</v>
+      </c>
+      <c r="H514" t="n">
+        <v>140</v>
+      </c>
+      <c r="I514" t="n">
+        <v>0</v>
+      </c>
+      <c r="J514" t="n">
+        <v>140</v>
+      </c>
+      <c r="K514" t="n">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>2021-12-11</t>
+        </is>
+      </c>
+      <c r="B515" t="n">
+        <v>9019</v>
+      </c>
+      <c r="C515" t="n">
+        <v>152</v>
+      </c>
+      <c r="D515" t="n">
+        <v>8867</v>
+      </c>
+      <c r="E515" t="n">
+        <v>3871</v>
+      </c>
+      <c r="F515" t="n">
+        <v>0</v>
+      </c>
+      <c r="G515" t="n">
+        <v>3871</v>
+      </c>
+      <c r="H515" t="n">
+        <v>140</v>
+      </c>
+      <c r="I515" t="n">
+        <v>0</v>
+      </c>
+      <c r="J515" t="n">
+        <v>140</v>
+      </c>
+      <c r="K515" t="n">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>2021-12-12</t>
+        </is>
+      </c>
+      <c r="B516" t="n">
+        <v>9019</v>
+      </c>
+      <c r="C516" t="n">
+        <v>153</v>
+      </c>
+      <c r="D516" t="n">
+        <v>8866</v>
+      </c>
+      <c r="E516" t="n">
+        <v>3871</v>
+      </c>
+      <c r="F516" t="n">
+        <v>0</v>
+      </c>
+      <c r="G516" t="n">
+        <v>3871</v>
+      </c>
+      <c r="H516" t="n">
+        <v>140</v>
+      </c>
+      <c r="I516" t="n">
+        <v>0</v>
+      </c>
+      <c r="J516" t="n">
+        <v>140</v>
+      </c>
+      <c r="K516" t="n">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>2021-12-13</t>
+        </is>
+      </c>
+      <c r="B517" t="n">
+        <v>8994</v>
+      </c>
+      <c r="C517" t="n">
+        <v>164</v>
+      </c>
+      <c r="D517" t="n">
+        <v>8830</v>
+      </c>
+      <c r="E517" t="n">
+        <v>3871</v>
+      </c>
+      <c r="F517" t="n">
+        <v>0</v>
+      </c>
+      <c r="G517" t="n">
+        <v>3871</v>
+      </c>
+      <c r="H517" t="n">
+        <v>140</v>
+      </c>
+      <c r="I517" t="n">
+        <v>0</v>
+      </c>
+      <c r="J517" t="n">
+        <v>140</v>
+      </c>
+      <c r="K517" t="n">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>2021-12-14</t>
+        </is>
+      </c>
+      <c r="B518" t="n">
+        <v>8994</v>
+      </c>
+      <c r="C518" t="n">
+        <v>169</v>
+      </c>
+      <c r="D518" t="n">
+        <v>8825</v>
+      </c>
+      <c r="E518" t="n">
+        <v>3871</v>
+      </c>
+      <c r="F518" t="n">
+        <v>0</v>
+      </c>
+      <c r="G518" t="n">
+        <v>3871</v>
+      </c>
+      <c r="H518" t="n">
+        <v>140</v>
+      </c>
+      <c r="I518" t="n">
+        <v>0</v>
+      </c>
+      <c r="J518" t="n">
+        <v>140</v>
+      </c>
+      <c r="K518" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>2021-12-15</t>
+        </is>
+      </c>
+      <c r="B519" t="n">
+        <v>8975</v>
+      </c>
+      <c r="C519" t="n">
+        <v>179</v>
+      </c>
+      <c r="D519" t="n">
+        <v>8796</v>
+      </c>
+      <c r="E519" t="n">
+        <v>3871</v>
+      </c>
+      <c r="F519" t="n">
+        <v>0</v>
+      </c>
+      <c r="G519" t="n">
+        <v>3871</v>
+      </c>
+      <c r="H519" t="n">
+        <v>140</v>
+      </c>
+      <c r="I519" t="n">
+        <v>0</v>
+      </c>
+      <c r="J519" t="n">
+        <v>140</v>
+      </c>
+      <c r="K519" t="n">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>2021-12-16</t>
+        </is>
+      </c>
+      <c r="B520" t="n">
+        <v>8987</v>
+      </c>
+      <c r="C520" t="n">
+        <v>188</v>
+      </c>
+      <c r="D520" t="n">
+        <v>8799</v>
+      </c>
+      <c r="E520" t="n">
+        <v>3871</v>
+      </c>
+      <c r="F520" t="n">
+        <v>0</v>
+      </c>
+      <c r="G520" t="n">
+        <v>3871</v>
+      </c>
+      <c r="H520" t="n">
+        <v>140</v>
+      </c>
+      <c r="I520" t="n">
+        <v>0</v>
+      </c>
+      <c r="J520" t="n">
+        <v>140</v>
+      </c>
+      <c r="K520" t="n">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>2021-12-17</t>
+        </is>
+      </c>
+      <c r="B521" t="n">
+        <v>8995</v>
+      </c>
+      <c r="C521" t="n">
+        <v>187</v>
+      </c>
+      <c r="D521" t="n">
+        <v>8808</v>
+      </c>
+      <c r="E521" t="n">
+        <v>3871</v>
+      </c>
+      <c r="F521" t="n">
+        <v>0</v>
+      </c>
+      <c r="G521" t="n">
+        <v>3871</v>
+      </c>
+      <c r="H521" t="n">
+        <v>140</v>
+      </c>
+      <c r="I521" t="n">
+        <v>0</v>
+      </c>
+      <c r="J521" t="n">
+        <v>140</v>
+      </c>
+      <c r="K521" t="n">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>2021-12-18</t>
+        </is>
+      </c>
+      <c r="B522" t="n">
+        <v>8995</v>
+      </c>
+      <c r="C522" t="n">
+        <v>195</v>
+      </c>
+      <c r="D522" t="n">
+        <v>8800</v>
+      </c>
+      <c r="E522" t="n">
+        <v>3871</v>
+      </c>
+      <c r="F522" t="n">
+        <v>0</v>
+      </c>
+      <c r="G522" t="n">
+        <v>3871</v>
+      </c>
+      <c r="H522" t="n">
+        <v>140</v>
+      </c>
+      <c r="I522" t="n">
+        <v>0</v>
+      </c>
+      <c r="J522" t="n">
+        <v>140</v>
+      </c>
+      <c r="K522" t="n">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>2021-12-19</t>
+        </is>
+      </c>
+      <c r="B523" t="n">
+        <v>8978</v>
+      </c>
+      <c r="C523" t="n">
+        <v>208</v>
+      </c>
+      <c r="D523" t="n">
+        <v>8770</v>
+      </c>
+      <c r="E523" t="n">
+        <v>3871</v>
+      </c>
+      <c r="F523" t="n">
+        <v>0</v>
+      </c>
+      <c r="G523" t="n">
+        <v>3871</v>
+      </c>
+      <c r="H523" t="n">
+        <v>140</v>
+      </c>
+      <c r="I523" t="n">
+        <v>0</v>
+      </c>
+      <c r="J523" t="n">
+        <v>140</v>
+      </c>
+      <c r="K523" t="n">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>2021-12-20</t>
+        </is>
+      </c>
+      <c r="B524" t="n">
+        <v>8975</v>
+      </c>
+      <c r="C524" t="n">
+        <v>197</v>
+      </c>
+      <c r="D524" t="n">
+        <v>8778</v>
+      </c>
+      <c r="E524" t="n">
+        <v>3871</v>
+      </c>
+      <c r="F524" t="n">
+        <v>0</v>
+      </c>
+      <c r="G524" t="n">
+        <v>3871</v>
+      </c>
+      <c r="H524" t="n">
+        <v>140</v>
+      </c>
+      <c r="I524" t="n">
+        <v>0</v>
+      </c>
+      <c r="J524" t="n">
+        <v>140</v>
+      </c>
+      <c r="K524" t="n">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>2021-12-21</t>
+        </is>
+      </c>
+      <c r="B525" t="n">
+        <v>9035</v>
+      </c>
+      <c r="C525" t="n">
+        <v>193</v>
+      </c>
+      <c r="D525" t="n">
+        <v>8842</v>
+      </c>
+      <c r="E525" t="n">
+        <v>3871</v>
+      </c>
+      <c r="F525" t="n">
+        <v>0</v>
+      </c>
+      <c r="G525" t="n">
+        <v>3871</v>
+      </c>
+      <c r="H525" t="n">
+        <v>140</v>
+      </c>
+      <c r="I525" t="n">
+        <v>0</v>
+      </c>
+      <c r="J525" t="n">
+        <v>140</v>
+      </c>
+      <c r="K525" t="n">
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -54627,7 +55863,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E464"/>
+  <dimension ref="A1:E476"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -63459,6 +64695,234 @@
       </c>
       <c r="E464" t="n">
         <v>1654568</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>2021-12-10</t>
+        </is>
+      </c>
+      <c r="B465" t="n">
+        <v>53174</v>
+      </c>
+      <c r="C465" t="n">
+        <v>6589</v>
+      </c>
+      <c r="D465" t="n">
+        <v>31496570</v>
+      </c>
+      <c r="E465" t="n">
+        <v>1657714</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>2021-12-11</t>
+        </is>
+      </c>
+      <c r="B466" t="n">
+        <v>50257</v>
+      </c>
+      <c r="C466" t="n">
+        <v>6887</v>
+      </c>
+      <c r="D466" t="n">
+        <v>31553714</v>
+      </c>
+      <c r="E466" t="n">
+        <v>1660721</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>2021-12-12</t>
+        </is>
+      </c>
+      <c r="B467" t="n">
+        <v>51263</v>
+      </c>
+      <c r="C467" t="n">
+        <v>5011</v>
+      </c>
+      <c r="D467" t="n">
+        <v>31609988</v>
+      </c>
+      <c r="E467" t="n">
+        <v>1663683</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>2021-12-13</t>
+        </is>
+      </c>
+      <c r="B468" t="n">
+        <v>43916</v>
+      </c>
+      <c r="C468" t="n">
+        <v>2253</v>
+      </c>
+      <c r="D468" t="n">
+        <v>31656157</v>
+      </c>
+      <c r="E468" t="n">
+        <v>1666113</v>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>2021-12-14</t>
+        </is>
+      </c>
+      <c r="B469" t="n">
+        <v>41734</v>
+      </c>
+      <c r="C469" t="n">
+        <v>6386</v>
+      </c>
+      <c r="D469" t="n">
+        <v>31704277</v>
+      </c>
+      <c r="E469" t="n">
+        <v>1668646</v>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>2021-12-15</t>
+        </is>
+      </c>
+      <c r="B470" t="n">
+        <v>52415</v>
+      </c>
+      <c r="C470" t="n">
+        <v>5913</v>
+      </c>
+      <c r="D470" t="n">
+        <v>31762605</v>
+      </c>
+      <c r="E470" t="n">
+        <v>1671716</v>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>2021-12-16</t>
+        </is>
+      </c>
+      <c r="B471" t="n">
+        <v>50879</v>
+      </c>
+      <c r="C471" t="n">
+        <v>5148</v>
+      </c>
+      <c r="D471" t="n">
+        <v>31818632</v>
+      </c>
+      <c r="E471" t="n">
+        <v>1674664</v>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>2021-12-17</t>
+        </is>
+      </c>
+      <c r="B472" t="n">
+        <v>51813</v>
+      </c>
+      <c r="C472" t="n">
+        <v>5485</v>
+      </c>
+      <c r="D472" t="n">
+        <v>31875930</v>
+      </c>
+      <c r="E472" t="n">
+        <v>1677680</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>2021-12-18</t>
+        </is>
+      </c>
+      <c r="B473" t="n">
+        <v>59901</v>
+      </c>
+      <c r="C473" t="n">
+        <v>6195</v>
+      </c>
+      <c r="D473" t="n">
+        <v>31942026</v>
+      </c>
+      <c r="E473" t="n">
+        <v>1681159</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>2021-12-19</t>
+        </is>
+      </c>
+      <c r="B474" t="n">
+        <v>57435</v>
+      </c>
+      <c r="C474" t="n">
+        <v>4470</v>
+      </c>
+      <c r="D474" t="n">
+        <v>32003931</v>
+      </c>
+      <c r="E474" t="n">
+        <v>1684417</v>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>2021-12-20</t>
+        </is>
+      </c>
+      <c r="B475" t="n">
+        <v>43917</v>
+      </c>
+      <c r="C475" t="n">
+        <v>2276</v>
+      </c>
+      <c r="D475" t="n">
+        <v>32050124</v>
+      </c>
+      <c r="E475" t="n">
+        <v>1686848</v>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>2021-12-21</t>
+        </is>
+      </c>
+      <c r="B476" t="n">
+        <v>45429</v>
+      </c>
+      <c r="C476" t="n">
+        <v>6115</v>
+      </c>
+      <c r="D476" t="n">
+        <v>32101668</v>
+      </c>
+      <c r="E476" t="n">
+        <v>1689561</v>
       </c>
     </row>
   </sheetData>
@@ -63472,7 +64936,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G230"/>
+  <dimension ref="A1:G242"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -69240,6 +70704,306 @@
       </c>
       <c r="G230" t="n">
         <v>9465998</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>2021-12-10</t>
+        </is>
+      </c>
+      <c r="B231" t="n">
+        <v>122300</v>
+      </c>
+      <c r="C231" t="n">
+        <v>48351</v>
+      </c>
+      <c r="D231" t="n">
+        <v>73949</v>
+      </c>
+      <c r="E231" t="n">
+        <v>23858032</v>
+      </c>
+      <c r="F231" t="n">
+        <v>14318085</v>
+      </c>
+      <c r="G231" t="n">
+        <v>9539947</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>2021-12-11</t>
+        </is>
+      </c>
+      <c r="B232" t="n">
+        <v>102660</v>
+      </c>
+      <c r="C232" t="n">
+        <v>39997</v>
+      </c>
+      <c r="D232" t="n">
+        <v>62663</v>
+      </c>
+      <c r="E232" t="n">
+        <v>23960692</v>
+      </c>
+      <c r="F232" t="n">
+        <v>14358082</v>
+      </c>
+      <c r="G232" t="n">
+        <v>9602610</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>2021-12-12</t>
+        </is>
+      </c>
+      <c r="B233" t="n">
+        <v>139453</v>
+      </c>
+      <c r="C233" t="n">
+        <v>49805</v>
+      </c>
+      <c r="D233" t="n">
+        <v>89648</v>
+      </c>
+      <c r="E233" t="n">
+        <v>24100145</v>
+      </c>
+      <c r="F233" t="n">
+        <v>14407887</v>
+      </c>
+      <c r="G233" t="n">
+        <v>9692258</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>2021-12-13</t>
+        </is>
+      </c>
+      <c r="B234" t="n">
+        <v>36072</v>
+      </c>
+      <c r="C234" t="n">
+        <v>15012</v>
+      </c>
+      <c r="D234" t="n">
+        <v>21060</v>
+      </c>
+      <c r="E234" t="n">
+        <v>24136217</v>
+      </c>
+      <c r="F234" t="n">
+        <v>14422899</v>
+      </c>
+      <c r="G234" t="n">
+        <v>9713318</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>2021-12-14</t>
+        </is>
+      </c>
+      <c r="B235" t="n">
+        <v>135262</v>
+      </c>
+      <c r="C235" t="n">
+        <v>49444</v>
+      </c>
+      <c r="D235" t="n">
+        <v>85818</v>
+      </c>
+      <c r="E235" t="n">
+        <v>24271479</v>
+      </c>
+      <c r="F235" t="n">
+        <v>14472343</v>
+      </c>
+      <c r="G235" t="n">
+        <v>9799136</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>2021-12-15</t>
+        </is>
+      </c>
+      <c r="B236" t="n">
+        <v>123434</v>
+      </c>
+      <c r="C236" t="n">
+        <v>45007</v>
+      </c>
+      <c r="D236" t="n">
+        <v>78427</v>
+      </c>
+      <c r="E236" t="n">
+        <v>24394913</v>
+      </c>
+      <c r="F236" t="n">
+        <v>14517350</v>
+      </c>
+      <c r="G236" t="n">
+        <v>9877563</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>2021-12-16</t>
+        </is>
+      </c>
+      <c r="B237" t="n">
+        <v>106902</v>
+      </c>
+      <c r="C237" t="n">
+        <v>38240</v>
+      </c>
+      <c r="D237" t="n">
+        <v>68662</v>
+      </c>
+      <c r="E237" t="n">
+        <v>24501815</v>
+      </c>
+      <c r="F237" t="n">
+        <v>14555590</v>
+      </c>
+      <c r="G237" t="n">
+        <v>9946225</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>2021-12-17</t>
+        </is>
+      </c>
+      <c r="B238" t="n">
+        <v>109221</v>
+      </c>
+      <c r="C238" t="n">
+        <v>37245</v>
+      </c>
+      <c r="D238" t="n">
+        <v>71976</v>
+      </c>
+      <c r="E238" t="n">
+        <v>24611036</v>
+      </c>
+      <c r="F238" t="n">
+        <v>14592835</v>
+      </c>
+      <c r="G238" t="n">
+        <v>10018201</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>2021-12-18</t>
+        </is>
+      </c>
+      <c r="B239" t="n">
+        <v>95460</v>
+      </c>
+      <c r="C239" t="n">
+        <v>31803</v>
+      </c>
+      <c r="D239" t="n">
+        <v>63657</v>
+      </c>
+      <c r="E239" t="n">
+        <v>24706496</v>
+      </c>
+      <c r="F239" t="n">
+        <v>14624638</v>
+      </c>
+      <c r="G239" t="n">
+        <v>10081858</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>2021-12-19</t>
+        </is>
+      </c>
+      <c r="B240" t="n">
+        <v>123719</v>
+      </c>
+      <c r="C240" t="n">
+        <v>38970</v>
+      </c>
+      <c r="D240" t="n">
+        <v>84749</v>
+      </c>
+      <c r="E240" t="n">
+        <v>24830215</v>
+      </c>
+      <c r="F240" t="n">
+        <v>14663608</v>
+      </c>
+      <c r="G240" t="n">
+        <v>10166607</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>2021-12-20</t>
+        </is>
+      </c>
+      <c r="B241" t="n">
+        <v>30080</v>
+      </c>
+      <c r="C241" t="n">
+        <v>11149</v>
+      </c>
+      <c r="D241" t="n">
+        <v>18931</v>
+      </c>
+      <c r="E241" t="n">
+        <v>24860295</v>
+      </c>
+      <c r="F241" t="n">
+        <v>14674757</v>
+      </c>
+      <c r="G241" t="n">
+        <v>10185538</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>2021-12-21</t>
+        </is>
+      </c>
+      <c r="B242" t="n">
+        <v>131180</v>
+      </c>
+      <c r="C242" t="n">
+        <v>41123</v>
+      </c>
+      <c r="D242" t="n">
+        <v>90057</v>
+      </c>
+      <c r="E242" t="n">
+        <v>24991475</v>
+      </c>
+      <c r="F242" t="n">
+        <v>14715880</v>
+      </c>
+      <c r="G242" t="n">
+        <v>10275595</v>
       </c>
     </row>
   </sheetData>

</xml_diff>